<commit_message>
new aggregations of euets permit allocation data
</commit_message>
<xml_diff>
--- a/_code/compilation/ecp/industry/4_euets/GLORIA_ISICr4.xlsx
+++ b/_code/compilation/ecp/industry/4_euets/GLORIA_ISICr4.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jomerkle\GitHub\ECP\_code\compilation\ecp\industry\4_euets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A08BB7-E647-4AAE-9E51-DC682E1236E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D2E3BBF-399D-4676-B7D6-E9E0AF0AAFB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sectors" sheetId="3" r:id="rId1"/>
     <sheet name="GLORIA to ISIC concordance" sheetId="9" r:id="rId2"/>
     <sheet name="GLORIA 97-to-120 concordance" sheetId="10" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" refMode="R1C1" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1096,9 +1096,6 @@
     <t>241; 243</t>
   </si>
   <si>
-    <t>241; 242</t>
-  </si>
-  <si>
     <t>2511; 2512; 2513; 2520; 2591; 2592; 2593; 2599</t>
   </si>
   <si>
@@ -1535,6 +1532,9 @@
   </si>
   <si>
     <t>2811; 2812; 2813; 2814; 2815; 2816; 2817; 2818; 2819; 2821; 2822; 2823; 2824; 2825; 2826; 2829</t>
+  </si>
+  <si>
+    <t>242; 243</t>
   </si>
 </sst>
 </file>
@@ -1941,8 +1941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="C88" sqref="C88"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1990,7 +1990,7 @@
         <v>266</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>273</v>
@@ -2010,7 +2010,7 @@
         <v>266</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>273</v>
@@ -2030,7 +2030,7 @@
         <v>266</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>273</v>
@@ -2050,7 +2050,7 @@
         <v>266</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>273</v>
@@ -2070,7 +2070,7 @@
         <v>266</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>273</v>
@@ -2090,7 +2090,7 @@
         <v>266</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>273</v>
@@ -2110,7 +2110,7 @@
         <v>266</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>273</v>
@@ -2130,7 +2130,7 @@
         <v>266</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>273</v>
@@ -2150,7 +2150,7 @@
         <v>266</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>273</v>
@@ -2170,7 +2170,7 @@
         <v>266</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>273</v>
@@ -2190,7 +2190,7 @@
         <v>265</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>273</v>
@@ -2210,7 +2210,7 @@
         <v>265</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>273</v>
@@ -2230,7 +2230,7 @@
         <v>265</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>273</v>
@@ -2250,7 +2250,7 @@
         <v>265</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>273</v>
@@ -2264,13 +2264,13 @@
         <v>16</v>
       </c>
       <c r="C16" s="4" t="s">
+        <v>455</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>456</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="E16" s="5" t="s">
         <v>457</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>458</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>273</v>
@@ -2290,7 +2290,7 @@
         <v>264</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>273</v>
@@ -2310,7 +2310,7 @@
         <v>264</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>273</v>
@@ -2330,7 +2330,7 @@
         <v>264</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>273</v>
@@ -2350,7 +2350,7 @@
         <v>264</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>273</v>
@@ -2370,7 +2370,7 @@
         <v>263</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>273</v>
@@ -2390,7 +2390,7 @@
         <v>267</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>273</v>
@@ -2410,7 +2410,7 @@
         <v>272</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>273</v>
@@ -2430,7 +2430,7 @@
         <v>270</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>273</v>
@@ -2450,7 +2450,7 @@
         <v>275</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>297</v>
@@ -2490,7 +2490,7 @@
         <v>280</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>297</v>
@@ -2510,7 +2510,7 @@
         <v>282</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>297</v>
@@ -2530,7 +2530,7 @@
         <v>284</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>297</v>
@@ -2550,7 +2550,7 @@
         <v>286</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>297</v>
@@ -2570,7 +2570,7 @@
         <v>286</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>297</v>
@@ -2590,7 +2590,7 @@
         <v>286</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>297</v>
@@ -2610,7 +2610,7 @@
         <v>286</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="F33" s="5" t="s">
         <v>297</v>
@@ -2630,7 +2630,7 @@
         <v>286</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>297</v>
@@ -2650,7 +2650,7 @@
         <v>286</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>297</v>
@@ -2670,7 +2670,7 @@
         <v>286</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="F36" s="5" t="s">
         <v>297</v>
@@ -2690,7 +2690,7 @@
         <v>286</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="F37" s="5" t="s">
         <v>297</v>
@@ -2710,7 +2710,7 @@
         <v>289</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>297</v>
@@ -2730,7 +2730,7 @@
         <v>292</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F39" s="5" t="s">
         <v>297</v>
@@ -2750,7 +2750,7 @@
         <v>292</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>297</v>
@@ -2790,7 +2790,7 @@
         <v>299</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="F42" s="5" t="s">
         <v>296</v>
@@ -2810,7 +2810,7 @@
         <v>299</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="F43" s="5" t="s">
         <v>296</v>
@@ -2830,7 +2830,7 @@
         <v>299</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>296</v>
@@ -2850,7 +2850,7 @@
         <v>299</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="F45" s="5" t="s">
         <v>296</v>
@@ -2870,7 +2870,7 @@
         <v>299</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="F46" s="5" t="s">
         <v>296</v>
@@ -2890,7 +2890,7 @@
         <v>301</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="F47" s="5" t="s">
         <v>296</v>
@@ -2910,7 +2910,7 @@
         <v>303</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="F48" s="5" t="s">
         <v>296</v>
@@ -2930,7 +2930,7 @@
         <v>305</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="F49" s="5" t="s">
         <v>296</v>
@@ -2950,7 +2950,7 @@
         <v>305</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="F50" s="5" t="s">
         <v>296</v>
@@ -2970,7 +2970,7 @@
         <v>313</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="F51" s="5" t="s">
         <v>296</v>
@@ -2990,7 +2990,7 @@
         <v>311</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="F52" s="5" t="s">
         <v>296</v>
@@ -3010,7 +3010,7 @@
         <v>307</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="F53" s="5" t="s">
         <v>296</v>
@@ -3030,7 +3030,7 @@
         <v>307</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="F54" s="5" t="s">
         <v>296</v>
@@ -3050,7 +3050,7 @@
         <v>309</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="F55" s="5" t="s">
         <v>296</v>
@@ -3070,7 +3070,7 @@
         <v>315</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="F56" s="5" t="s">
         <v>296</v>
@@ -3090,7 +3090,7 @@
         <v>317</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="F57" s="5" t="s">
         <v>296</v>
@@ -3130,7 +3130,7 @@
         <v>322</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="F59" s="5" t="s">
         <v>296</v>
@@ -3150,7 +3150,7 @@
         <v>324</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="F60" s="5" t="s">
         <v>296</v>
@@ -3170,7 +3170,7 @@
         <v>326</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="F61" s="5" t="s">
         <v>296</v>
@@ -3190,7 +3190,7 @@
         <v>328</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F62" s="5" t="s">
         <v>296</v>
@@ -3210,7 +3210,7 @@
         <v>330</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="F63" s="5" t="s">
         <v>296</v>
@@ -3230,7 +3230,7 @@
         <v>332</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="F64" s="5" t="s">
         <v>296</v>
@@ -3250,7 +3250,7 @@
         <v>335</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="F65" s="5" t="s">
         <v>296</v>
@@ -3270,7 +3270,7 @@
         <v>337</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="F66" s="5" t="s">
         <v>296</v>
@@ -3284,13 +3284,13 @@
         <v>67</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D67" s="5" t="s">
         <v>335</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="F67" s="5" t="s">
         <v>296</v>
@@ -3310,7 +3310,7 @@
         <v>335</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="F68" s="5" t="s">
         <v>296</v>
@@ -3330,7 +3330,7 @@
         <v>335</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="F69" s="5" t="s">
         <v>296</v>
@@ -3350,7 +3350,7 @@
         <v>339</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F70" s="5" t="s">
         <v>296</v>
@@ -3364,13 +3364,13 @@
         <v>71</v>
       </c>
       <c r="C71" s="4" t="s">
+        <v>496</v>
+      </c>
+      <c r="D71" s="5" t="s">
         <v>497</v>
       </c>
-      <c r="D71" s="5" t="s">
-        <v>498</v>
-      </c>
       <c r="E71" s="5" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="F71" s="5" t="s">
         <v>296</v>
@@ -3390,7 +3390,7 @@
         <v>341</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="F72" s="5" t="s">
         <v>296</v>
@@ -3410,7 +3410,7 @@
         <v>343</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="F73" s="5" t="s">
         <v>296</v>
@@ -3430,7 +3430,7 @@
         <v>345</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="F74" s="5" t="s">
         <v>296</v>
@@ -3450,7 +3450,7 @@
         <v>349</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="F75" s="5" t="s">
         <v>296</v>
@@ -3470,7 +3470,7 @@
         <v>345</v>
       </c>
       <c r="E76" s="5" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="F76" s="5" t="s">
         <v>296</v>
@@ -3490,7 +3490,7 @@
         <v>345</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="F77" s="5" t="s">
         <v>296</v>
@@ -3510,7 +3510,7 @@
         <v>352</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="F78" s="5" t="s">
         <v>296</v>
@@ -3527,10 +3527,10 @@
         <v>351</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>353</v>
+        <v>499</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="F79" s="5" t="s">
         <v>296</v>
@@ -3547,10 +3547,10 @@
         <v>351</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>353</v>
+        <v>499</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="F80" s="5" t="s">
         <v>296</v>
@@ -3567,10 +3567,10 @@
         <v>351</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>353</v>
+        <v>499</v>
       </c>
       <c r="E81" s="5" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="F81" s="5" t="s">
         <v>296</v>
@@ -3587,10 +3587,10 @@
         <v>351</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>353</v>
+        <v>499</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="F82" s="5" t="s">
         <v>296</v>
@@ -3607,10 +3607,10 @@
         <v>351</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>353</v>
+        <v>499</v>
       </c>
       <c r="E83" s="5" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="F83" s="5" t="s">
         <v>296</v>
@@ -3627,10 +3627,10 @@
         <v>351</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>353</v>
+        <v>499</v>
       </c>
       <c r="E84" s="5" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="F84" s="5" t="s">
         <v>296</v>
@@ -3647,10 +3647,10 @@
         <v>351</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>353</v>
+        <v>499</v>
       </c>
       <c r="E85" s="5" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="F85" s="5" t="s">
         <v>296</v>
@@ -3664,13 +3664,13 @@
         <v>86</v>
       </c>
       <c r="C86" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="D86" s="5" t="s">
         <v>354</v>
       </c>
-      <c r="D86" s="5" t="s">
-        <v>355</v>
-      </c>
       <c r="E86" s="5" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="F86" s="5" t="s">
         <v>296</v>
@@ -3684,13 +3684,13 @@
         <v>87</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="F87" s="5" t="s">
         <v>296</v>
@@ -3704,13 +3704,13 @@
         <v>88</v>
       </c>
       <c r="C88" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="D88" s="5" t="s">
         <v>361</v>
       </c>
-      <c r="D88" s="5" t="s">
-        <v>362</v>
-      </c>
       <c r="E88" s="5" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="F88" s="5" t="s">
         <v>296</v>
@@ -3724,13 +3724,13 @@
         <v>89</v>
       </c>
       <c r="C89" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="D89" s="5" t="s">
         <v>363</v>
       </c>
-      <c r="D89" s="5" t="s">
-        <v>364</v>
-      </c>
       <c r="E89" s="5" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="F89" s="5" t="s">
         <v>296</v>
@@ -3744,13 +3744,13 @@
         <v>90</v>
       </c>
       <c r="C90" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="D90" s="5" t="s">
         <v>368</v>
       </c>
-      <c r="D90" s="5" t="s">
-        <v>369</v>
-      </c>
       <c r="E90" s="5" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="F90" s="5" t="s">
         <v>296</v>
@@ -3764,13 +3764,13 @@
         <v>91</v>
       </c>
       <c r="C91" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="D91" s="5" t="s">
         <v>356</v>
       </c>
-      <c r="D91" s="5" t="s">
-        <v>357</v>
-      </c>
       <c r="E91" s="5" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F91" s="5" t="s">
         <v>296</v>
@@ -3784,13 +3784,13 @@
         <v>92</v>
       </c>
       <c r="C92" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="D92" s="5" t="s">
         <v>358</v>
       </c>
-      <c r="D92" s="5" t="s">
-        <v>359</v>
-      </c>
       <c r="E92" s="5" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="F92" s="5" t="s">
         <v>296</v>
@@ -3804,13 +3804,13 @@
         <v>93</v>
       </c>
       <c r="C93" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="D93" s="5" t="s">
         <v>365</v>
       </c>
-      <c r="D93" s="5" t="s">
+      <c r="E93" s="5" t="s">
         <v>366</v>
-      </c>
-      <c r="E93" s="5" t="s">
-        <v>367</v>
       </c>
       <c r="F93" s="5" t="s">
         <v>296</v>
@@ -3824,16 +3824,16 @@
         <v>94</v>
       </c>
       <c r="C94" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="D94" s="5" t="s">
         <v>370</v>
       </c>
-      <c r="D94" s="5" t="s">
-        <v>371</v>
-      </c>
       <c r="E94" s="5" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="F94" s="5" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -3844,16 +3844,16 @@
         <v>95</v>
       </c>
       <c r="C95" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="D95" s="5" t="s">
         <v>372</v>
       </c>
-      <c r="D95" s="5" t="s">
-        <v>373</v>
-      </c>
       <c r="E95" s="5" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="F95" s="5" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="96" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
@@ -3864,16 +3864,16 @@
         <v>96</v>
       </c>
       <c r="C96" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="D96" s="5" t="s">
         <v>374</v>
       </c>
-      <c r="D96" s="5" t="s">
+      <c r="E96" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="E96" s="5" t="s">
-        <v>376</v>
-      </c>
       <c r="F96" s="5" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="97" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
@@ -3884,16 +3884,16 @@
         <v>97</v>
       </c>
       <c r="C97" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="D97" s="5" t="s">
         <v>381</v>
       </c>
-      <c r="D97" s="5" t="s">
+      <c r="E97" s="5" t="s">
         <v>382</v>
       </c>
-      <c r="E97" s="5" t="s">
-        <v>383</v>
-      </c>
       <c r="F97" s="5" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
@@ -3904,16 +3904,16 @@
         <v>98</v>
       </c>
       <c r="C98" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="D98" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="D98" s="5" t="s">
+      <c r="E98" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="F98" s="5" t="s">
         <v>378</v>
-      </c>
-      <c r="E98" s="5" t="s">
-        <v>486</v>
-      </c>
-      <c r="F98" s="5" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="99" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -3924,16 +3924,16 @@
         <v>99</v>
       </c>
       <c r="C99" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="D99" s="5" t="s">
         <v>385</v>
       </c>
-      <c r="D99" s="5" t="s">
+      <c r="E99" s="5" t="s">
         <v>386</v>
       </c>
-      <c r="E99" s="5" t="s">
-        <v>387</v>
-      </c>
       <c r="F99" s="5" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="100" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -3944,16 +3944,16 @@
         <v>100</v>
       </c>
       <c r="C100" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="D100" s="5" t="s">
         <v>388</v>
       </c>
-      <c r="D100" s="5" t="s">
+      <c r="E100" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="E100" s="5" t="s">
-        <v>390</v>
-      </c>
       <c r="F100" s="5" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="101" spans="1:6" ht="87" x14ac:dyDescent="0.35">
@@ -3964,16 +3964,16 @@
         <v>101</v>
       </c>
       <c r="C101" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="D101" s="5" t="s">
         <v>392</v>
       </c>
-      <c r="D101" s="5" t="s">
+      <c r="E101" s="5" t="s">
         <v>393</v>
       </c>
-      <c r="E101" s="5" t="s">
-        <v>394</v>
-      </c>
       <c r="F101" s="5" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.35">
@@ -3984,16 +3984,16 @@
         <v>102</v>
       </c>
       <c r="C102" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="D102" s="5" t="s">
         <v>398</v>
       </c>
-      <c r="D102" s="5" t="s">
-        <v>399</v>
-      </c>
       <c r="E102" s="5" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="F102" s="5" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.35">
@@ -4004,16 +4004,16 @@
         <v>103</v>
       </c>
       <c r="C103" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="D103" s="5" t="s">
         <v>395</v>
       </c>
-      <c r="D103" s="5" t="s">
+      <c r="E103" s="5" t="s">
+        <v>486</v>
+      </c>
+      <c r="F103" s="5" t="s">
         <v>396</v>
-      </c>
-      <c r="E103" s="5" t="s">
-        <v>487</v>
-      </c>
-      <c r="F103" s="5" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.35">
@@ -4024,16 +4024,16 @@
         <v>104</v>
       </c>
       <c r="C104" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="D104" s="5" t="s">
         <v>400</v>
       </c>
-      <c r="D104" s="5" t="s">
-        <v>401</v>
-      </c>
       <c r="E104" s="5" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="F104" s="5" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.35">
@@ -4044,16 +4044,16 @@
         <v>105</v>
       </c>
       <c r="C105" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="D105" s="5" t="s">
         <v>402</v>
       </c>
-      <c r="D105" s="5" t="s">
-        <v>403</v>
-      </c>
       <c r="E105" s="5" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="F105" s="5" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.35">
@@ -4064,16 +4064,16 @@
         <v>106</v>
       </c>
       <c r="C106" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="D106" s="5" t="s">
         <v>404</v>
       </c>
-      <c r="D106" s="5" t="s">
-        <v>405</v>
-      </c>
       <c r="E106" s="5" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="F106" s="5" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.35">
@@ -4084,16 +4084,16 @@
         <v>107</v>
       </c>
       <c r="C107" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="D107" s="5" t="s">
         <v>406</v>
       </c>
-      <c r="D107" s="5" t="s">
-        <v>407</v>
-      </c>
       <c r="E107" s="5" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="F107" s="5" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.35">
@@ -4104,16 +4104,16 @@
         <v>108</v>
       </c>
       <c r="C108" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="D108" s="5" t="s">
         <v>408</v>
       </c>
-      <c r="D108" s="5" t="s">
-        <v>409</v>
-      </c>
       <c r="E108" s="5" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F108" s="5" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="109" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -4124,16 +4124,16 @@
         <v>109</v>
       </c>
       <c r="C109" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="D109" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="D109" s="5" t="s">
+      <c r="E109" s="5" t="s">
         <v>411</v>
       </c>
-      <c r="E109" s="5" t="s">
+      <c r="F109" s="5" t="s">
         <v>412</v>
-      </c>
-      <c r="F109" s="5" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="110" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -4144,16 +4144,16 @@
         <v>110</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D110" s="5" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E110" s="5" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="F110" s="5" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.35">
@@ -4164,16 +4164,16 @@
         <v>111</v>
       </c>
       <c r="C111" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="D111" s="5" t="s">
         <v>418</v>
       </c>
-      <c r="D111" s="5" t="s">
-        <v>419</v>
-      </c>
       <c r="E111" s="5" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="F111" s="5" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.35">
@@ -4184,16 +4184,16 @@
         <v>112</v>
       </c>
       <c r="C112" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="D112" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="E112" s="5" t="s">
         <v>421</v>
       </c>
-      <c r="D112" s="5" t="s">
-        <v>420</v>
-      </c>
-      <c r="E112" s="5" t="s">
-        <v>422</v>
-      </c>
       <c r="F112" s="5" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="113" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
@@ -4204,16 +4204,16 @@
         <v>113</v>
       </c>
       <c r="C113" s="4" t="s">
+        <v>422</v>
+      </c>
+      <c r="D113" s="5" t="s">
         <v>423</v>
       </c>
-      <c r="D113" s="5" t="s">
+      <c r="E113" s="5" t="s">
         <v>424</v>
       </c>
-      <c r="E113" s="5" t="s">
+      <c r="F113" s="5" t="s">
         <v>425</v>
-      </c>
-      <c r="F113" s="5" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.35">
@@ -4224,16 +4224,16 @@
         <v>114</v>
       </c>
       <c r="C114" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="D114" s="5" t="s">
         <v>427</v>
       </c>
-      <c r="D114" s="5" t="s">
+      <c r="E114" s="5" t="s">
+        <v>492</v>
+      </c>
+      <c r="F114" s="5" t="s">
         <v>428</v>
-      </c>
-      <c r="E114" s="5" t="s">
-        <v>493</v>
-      </c>
-      <c r="F114" s="5" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="115" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -4244,16 +4244,16 @@
         <v>115</v>
       </c>
       <c r="C115" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="D115" s="5" t="s">
         <v>432</v>
       </c>
-      <c r="D115" s="5" t="s">
-        <v>433</v>
-      </c>
       <c r="E115" s="5" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F115" s="5" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="116" spans="1:6" ht="58" x14ac:dyDescent="0.35">
@@ -4264,16 +4264,16 @@
         <v>116</v>
       </c>
       <c r="C116" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="D116" s="5" t="s">
         <v>444</v>
       </c>
-      <c r="D116" s="5" t="s">
-        <v>445</v>
-      </c>
       <c r="E116" s="5" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F116" s="5" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="117" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -4284,16 +4284,16 @@
         <v>117</v>
       </c>
       <c r="C117" s="4" t="s">
+        <v>445</v>
+      </c>
+      <c r="D117" s="5" t="s">
         <v>446</v>
       </c>
-      <c r="D117" s="5" t="s">
-        <v>447</v>
-      </c>
       <c r="E117" s="5" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F117" s="5" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="118" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -4304,16 +4304,16 @@
         <v>118</v>
       </c>
       <c r="C118" s="4" t="s">
+        <v>447</v>
+      </c>
+      <c r="D118" s="5" t="s">
         <v>448</v>
       </c>
-      <c r="D118" s="5" t="s">
-        <v>449</v>
-      </c>
       <c r="E118" s="5" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="F118" s="5" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="119" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -4324,16 +4324,16 @@
         <v>119</v>
       </c>
       <c r="C119" s="4" t="s">
+        <v>449</v>
+      </c>
+      <c r="D119" s="5" t="s">
         <v>450</v>
       </c>
-      <c r="D119" s="5" t="s">
-        <v>451</v>
-      </c>
       <c r="E119" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="F119" s="5" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="120" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -4344,16 +4344,16 @@
         <v>120</v>
       </c>
       <c r="C120" s="4" t="s">
+        <v>451</v>
+      </c>
+      <c r="D120" s="5" t="s">
         <v>452</v>
       </c>
-      <c r="D120" s="5" t="s">
-        <v>453</v>
-      </c>
       <c r="E120" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="F120" s="5" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="121" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
@@ -4364,16 +4364,16 @@
         <v>121</v>
       </c>
       <c r="C121" s="4" t="s">
+        <v>453</v>
+      </c>
+      <c r="D121" s="5" t="s">
         <v>454</v>
       </c>
-      <c r="D121" s="5" t="s">
-        <v>455</v>
-      </c>
       <c r="E121" s="5" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="F121" s="5" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
   </sheetData>

</xml_diff>